<commit_message>
- Cập nhật bản phân tích chức năng basic design
</commit_message>
<xml_diff>
--- a/Wip/Documents/java-s/InterfaceAnalysis/Nghia.InterfaceAnalysis.xlsx
+++ b/Wip/Documents/java-s/InterfaceAnalysis/Nghia.InterfaceAnalysis.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="135" windowWidth="18195" windowHeight="8505" tabRatio="874" firstSheet="9" activeTab="10"/>
+    <workbookView xWindow="480" yWindow="135" windowWidth="18195" windowHeight="8505" tabRatio="874" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Chien_OrgList" sheetId="1" r:id="rId1"/>
@@ -23,9 +23,101 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="28">
+  <si>
+    <t>Process ID</t>
+  </si>
+  <si>
+    <t>Process name</t>
+  </si>
+  <si>
+    <t>Function name</t>
+  </si>
+  <si>
+    <t>Format run (gọi ra)</t>
+  </si>
+  <si>
+    <t>Tham số</t>
+  </si>
+  <si>
+    <t>Output kết quả run</t>
+  </si>
+  <si>
+    <t>Giá trị trả về</t>
+  </si>
+  <si>
+    <t>Process nguồn gọi ra</t>
+  </si>
+  <si>
+    <t>（Process ID）</t>
+  </si>
+  <si>
+    <t>amend_org</t>
+  </si>
+  <si>
+    <t>Liệt kê các Premise liên kết với Organisation</t>
+  </si>
+  <si>
+    <t>[th.so1],[th.so2],[th.so3],[th.so4],[th.so5]</t>
+  </si>
+  <si>
+    <t>Ward, Borough, Local Authority, Unitry Authority, NHS Authority chỉ đọc</t>
+  </si>
+  <si>
+    <t>hiển thị các trường ra màn hình</t>
+  </si>
+  <si>
+    <t>SubSystem</t>
+  </si>
+  <si>
+    <t>Create date</t>
+  </si>
+  <si>
+    <t>Update date</t>
+  </si>
+  <si>
+    <t>Giải thích chức năng</t>
+  </si>
+  <si>
+    <t>Hiển thị thông tin một active premises</t>
+  </si>
+  <si>
+    <t>【Nội dung xử lý】</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SQL: Select * from Premise  </t>
+  </si>
+  <si>
+    <t>SupOrg</t>
+  </si>
+  <si>
+    <t>geSupOrg[tham so]</t>
+  </si>
+  <si>
+    <t>các thuộc tính trong bảng SupportingMaterial</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SQL: Select * from SupportingMaterial  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nếu xảy ra lỗi thì thông báo </t>
+  </si>
+  <si>
+    <t>Hiển thị thông tin một Supporting Material</t>
+  </si>
+  <si>
+    <t>true : save thành công/ false : save thất bại</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="\(0\)"/>
+  </numFmts>
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -33,16 +125,27 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="22"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="35">
     <border>
       <left/>
       <right/>
@@ -50,12 +153,561 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -417,16 +1069,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>605117</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>22412</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>448310</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>11430</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>67236</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>145676</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -442,8 +1094,8 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="609600" y="762000"/>
-          <a:ext cx="5934710" cy="1535430"/>
+          <a:off x="605117" y="212912"/>
+          <a:ext cx="7328648" cy="2790264"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -928,7 +1580,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
@@ -986,14 +1638,412 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="B22:V37"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I25" sqref="I25"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E28" sqref="E28:M28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="22" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="23" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B23" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="C23" s="14"/>
+      <c r="D23" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="E23" s="13"/>
+      <c r="F23" s="13"/>
+      <c r="G23" s="14"/>
+      <c r="H23" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="I23" s="13"/>
+      <c r="J23" s="13"/>
+      <c r="K23" s="13"/>
+      <c r="L23" s="13"/>
+      <c r="M23" s="14"/>
+      <c r="N23" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="O23" s="13"/>
+      <c r="P23" s="13"/>
+      <c r="Q23" s="13"/>
+      <c r="R23" s="14"/>
+      <c r="S23" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="T23" s="14"/>
+      <c r="U23" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="V23" s="14"/>
+    </row>
+    <row r="24" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B24" s="24"/>
+      <c r="C24" s="26"/>
+      <c r="D24" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="E24" s="25"/>
+      <c r="F24" s="25"/>
+      <c r="G24" s="26"/>
+      <c r="H24" s="24" t="s">
+        <v>10</v>
+      </c>
+      <c r="I24" s="25"/>
+      <c r="J24" s="25"/>
+      <c r="K24" s="25"/>
+      <c r="L24" s="25"/>
+      <c r="M24" s="26"/>
+      <c r="N24" s="24"/>
+      <c r="O24" s="25"/>
+      <c r="P24" s="25"/>
+      <c r="Q24" s="25"/>
+      <c r="R24" s="26"/>
+      <c r="S24" s="24"/>
+      <c r="T24" s="26"/>
+      <c r="U24" s="24"/>
+      <c r="V24" s="26"/>
+    </row>
+    <row r="25" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B25" s="42" t="s">
+        <v>3</v>
+      </c>
+      <c r="C25" s="43"/>
+      <c r="D25" s="44"/>
+      <c r="E25" s="45" t="s">
+        <v>11</v>
+      </c>
+      <c r="F25" s="46"/>
+      <c r="G25" s="46"/>
+      <c r="H25" s="46"/>
+      <c r="I25" s="46"/>
+      <c r="J25" s="46"/>
+      <c r="K25" s="46"/>
+      <c r="L25" s="46"/>
+      <c r="M25" s="47"/>
+      <c r="N25" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="O25" s="13"/>
+      <c r="P25" s="13"/>
+      <c r="Q25" s="13"/>
+      <c r="R25" s="13"/>
+      <c r="S25" s="13"/>
+      <c r="T25" s="13"/>
+      <c r="U25" s="13"/>
+      <c r="V25" s="14"/>
+    </row>
+    <row r="26" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B26" s="48" t="s">
+        <v>4</v>
+      </c>
+      <c r="C26" s="49"/>
+      <c r="D26" s="50"/>
+      <c r="E26" s="51" t="s">
+        <v>12</v>
+      </c>
+      <c r="F26" s="52"/>
+      <c r="G26" s="52"/>
+      <c r="H26" s="52"/>
+      <c r="I26" s="52"/>
+      <c r="J26" s="52"/>
+      <c r="K26" s="52"/>
+      <c r="L26" s="52"/>
+      <c r="M26" s="53"/>
+      <c r="N26" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="O26" s="16"/>
+      <c r="P26" s="16"/>
+      <c r="Q26" s="16"/>
+      <c r="R26" s="16"/>
+      <c r="S26" s="16"/>
+      <c r="T26" s="16"/>
+      <c r="U26" s="16"/>
+      <c r="V26" s="17"/>
+    </row>
+    <row r="27" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B27" s="48" t="s">
+        <v>5</v>
+      </c>
+      <c r="C27" s="49"/>
+      <c r="D27" s="50"/>
+      <c r="E27" s="51" t="s">
+        <v>13</v>
+      </c>
+      <c r="F27" s="52"/>
+      <c r="G27" s="52"/>
+      <c r="H27" s="52"/>
+      <c r="I27" s="52"/>
+      <c r="J27" s="52"/>
+      <c r="K27" s="52"/>
+      <c r="L27" s="52"/>
+      <c r="M27" s="53"/>
+      <c r="N27" s="18"/>
+      <c r="O27" s="19"/>
+      <c r="P27" s="19"/>
+      <c r="Q27" s="19"/>
+      <c r="R27" s="19"/>
+      <c r="S27" s="19"/>
+      <c r="T27" s="19"/>
+      <c r="U27" s="19"/>
+      <c r="V27" s="20"/>
+    </row>
+    <row r="28" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B28" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="C28" s="28"/>
+      <c r="D28" s="29"/>
+      <c r="E28" s="30" t="s">
+        <v>27</v>
+      </c>
+      <c r="F28" s="31"/>
+      <c r="G28" s="31"/>
+      <c r="H28" s="31"/>
+      <c r="I28" s="31"/>
+      <c r="J28" s="31"/>
+      <c r="K28" s="31"/>
+      <c r="L28" s="31"/>
+      <c r="M28" s="32"/>
+      <c r="N28" s="18"/>
+      <c r="O28" s="19"/>
+      <c r="P28" s="19"/>
+      <c r="Q28" s="19"/>
+      <c r="R28" s="19"/>
+      <c r="S28" s="19"/>
+      <c r="T28" s="19"/>
+      <c r="U28" s="19"/>
+      <c r="V28" s="20"/>
+    </row>
+    <row r="29" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B29" s="33" t="s">
+        <v>7</v>
+      </c>
+      <c r="C29" s="34"/>
+      <c r="D29" s="35"/>
+      <c r="E29" s="36"/>
+      <c r="F29" s="37"/>
+      <c r="G29" s="37"/>
+      <c r="H29" s="38"/>
+      <c r="I29" s="39" t="s">
+        <v>8</v>
+      </c>
+      <c r="J29" s="34"/>
+      <c r="K29" s="35"/>
+      <c r="L29" s="40"/>
+      <c r="M29" s="41"/>
+      <c r="N29" s="21"/>
+      <c r="O29" s="22"/>
+      <c r="P29" s="22"/>
+      <c r="Q29" s="22"/>
+      <c r="R29" s="22"/>
+      <c r="S29" s="22"/>
+      <c r="T29" s="22"/>
+      <c r="U29" s="22"/>
+      <c r="V29" s="23"/>
+    </row>
+    <row r="31" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B31" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C31" s="1"/>
+      <c r="D31" s="1"/>
+      <c r="E31" s="1"/>
+      <c r="F31" s="1"/>
+      <c r="G31" s="1"/>
+      <c r="H31" s="1"/>
+      <c r="I31" s="1"/>
+      <c r="J31" s="1"/>
+      <c r="K31" s="1"/>
+      <c r="L31" s="1"/>
+      <c r="M31" s="1"/>
+      <c r="N31" s="1"/>
+      <c r="O31" s="1"/>
+      <c r="P31" s="1"/>
+      <c r="Q31" s="1"/>
+      <c r="R31" s="1"/>
+      <c r="S31" s="1"/>
+      <c r="T31" s="1"/>
+      <c r="U31" s="1"/>
+      <c r="V31" s="1"/>
+    </row>
+    <row r="32" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B32" s="2"/>
+      <c r="C32" s="3"/>
+      <c r="D32" s="3"/>
+      <c r="E32" s="3"/>
+      <c r="F32" s="3"/>
+      <c r="G32" s="3"/>
+      <c r="H32" s="3"/>
+      <c r="I32" s="3"/>
+      <c r="J32" s="3"/>
+      <c r="K32" s="3"/>
+      <c r="L32" s="3"/>
+      <c r="M32" s="3"/>
+      <c r="N32" s="3"/>
+      <c r="O32" s="3"/>
+      <c r="P32" s="3"/>
+      <c r="Q32" s="3"/>
+      <c r="R32" s="3"/>
+      <c r="S32" s="3"/>
+      <c r="T32" s="3"/>
+      <c r="U32" s="3"/>
+      <c r="V32" s="4"/>
+    </row>
+    <row r="33" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B33" s="5"/>
+      <c r="C33" s="6">
+        <v>1</v>
+      </c>
+      <c r="D33" t="s">
+        <v>20</v>
+      </c>
+      <c r="E33" s="7"/>
+      <c r="F33" s="7"/>
+      <c r="G33" s="7"/>
+      <c r="H33" s="7"/>
+      <c r="I33" s="7"/>
+      <c r="J33" s="7"/>
+      <c r="K33" s="7"/>
+      <c r="L33" s="7"/>
+      <c r="M33" s="7"/>
+      <c r="N33" s="7"/>
+      <c r="O33" s="7"/>
+      <c r="P33" s="7"/>
+      <c r="Q33" s="7"/>
+      <c r="R33" s="7"/>
+      <c r="S33" s="7"/>
+      <c r="T33" s="7"/>
+      <c r="U33" s="7"/>
+      <c r="V33" s="8"/>
+    </row>
+    <row r="34" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B34" s="5"/>
+      <c r="C34" s="6"/>
+      <c r="D34" s="7"/>
+      <c r="E34" s="7"/>
+      <c r="F34" s="7"/>
+      <c r="G34" s="7"/>
+      <c r="H34" s="7"/>
+      <c r="I34" s="7"/>
+      <c r="J34" s="7"/>
+      <c r="K34" s="7"/>
+      <c r="L34" s="7"/>
+      <c r="M34" s="7"/>
+      <c r="N34" s="7"/>
+      <c r="O34" s="7"/>
+      <c r="P34" s="7"/>
+      <c r="Q34" s="7"/>
+      <c r="R34" s="7"/>
+      <c r="S34" s="7"/>
+      <c r="T34" s="7"/>
+      <c r="U34" s="7"/>
+      <c r="V34" s="8"/>
+    </row>
+    <row r="35" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B35" s="5"/>
+      <c r="C35" s="6"/>
+      <c r="D35" s="7"/>
+      <c r="E35" s="7"/>
+      <c r="F35" s="7"/>
+      <c r="G35" s="7"/>
+      <c r="H35" s="7"/>
+      <c r="I35" s="7"/>
+      <c r="J35" s="7"/>
+      <c r="K35" s="7"/>
+      <c r="L35" s="7"/>
+      <c r="M35" s="7"/>
+      <c r="N35" s="7"/>
+      <c r="O35" s="7"/>
+      <c r="P35" s="7"/>
+      <c r="Q35" s="7"/>
+      <c r="R35" s="7"/>
+      <c r="S35" s="7"/>
+      <c r="T35" s="7"/>
+      <c r="U35" s="7"/>
+      <c r="V35" s="8"/>
+    </row>
+    <row r="36" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B36" s="5"/>
+      <c r="C36" s="6"/>
+      <c r="D36" s="7"/>
+      <c r="E36" s="7"/>
+      <c r="F36" s="7"/>
+      <c r="G36" s="7"/>
+      <c r="H36" s="7"/>
+      <c r="I36" s="7"/>
+      <c r="J36" s="7"/>
+      <c r="K36" s="7"/>
+      <c r="L36" s="7"/>
+      <c r="M36" s="7"/>
+      <c r="N36" s="7"/>
+      <c r="O36" s="7"/>
+      <c r="P36" s="7"/>
+      <c r="Q36" s="7"/>
+      <c r="R36" s="7"/>
+      <c r="S36" s="7"/>
+      <c r="T36" s="7"/>
+      <c r="U36" s="7"/>
+      <c r="V36" s="8"/>
+    </row>
+    <row r="37" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B37" s="9"/>
+      <c r="C37" s="10"/>
+      <c r="D37" s="10"/>
+      <c r="E37" s="10"/>
+      <c r="F37" s="10"/>
+      <c r="G37" s="10"/>
+      <c r="H37" s="10"/>
+      <c r="I37" s="10"/>
+      <c r="J37" s="10"/>
+      <c r="K37" s="10"/>
+      <c r="L37" s="10"/>
+      <c r="M37" s="10"/>
+      <c r="N37" s="10"/>
+      <c r="O37" s="10"/>
+      <c r="P37" s="10"/>
+      <c r="Q37" s="10"/>
+      <c r="R37" s="10"/>
+      <c r="S37" s="10"/>
+      <c r="T37" s="10"/>
+      <c r="U37" s="10"/>
+      <c r="V37" s="11"/>
+    </row>
+  </sheetData>
+  <mergeCells count="26">
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="D23:G23"/>
+    <mergeCell ref="H23:M23"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="D24:G24"/>
+    <mergeCell ref="H24:M24"/>
+    <mergeCell ref="B25:D25"/>
+    <mergeCell ref="E25:M25"/>
+    <mergeCell ref="B26:D26"/>
+    <mergeCell ref="E26:M26"/>
+    <mergeCell ref="B27:D27"/>
+    <mergeCell ref="E27:M27"/>
+    <mergeCell ref="B28:D28"/>
+    <mergeCell ref="E28:M28"/>
+    <mergeCell ref="B29:D29"/>
+    <mergeCell ref="E29:H29"/>
+    <mergeCell ref="I29:K29"/>
+    <mergeCell ref="L29:M29"/>
+    <mergeCell ref="N25:V25"/>
+    <mergeCell ref="N26:V29"/>
+    <mergeCell ref="N23:R23"/>
+    <mergeCell ref="S23:T23"/>
+    <mergeCell ref="U23:V23"/>
+    <mergeCell ref="N24:R24"/>
+    <mergeCell ref="S24:T24"/>
+    <mergeCell ref="U24:V24"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
@@ -1001,14 +2051,412 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="B19:V34"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="J31" sqref="J31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="19" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="20" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B20" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="C20" s="14"/>
+      <c r="D20" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="E20" s="13"/>
+      <c r="F20" s="13"/>
+      <c r="G20" s="14"/>
+      <c r="H20" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="I20" s="13"/>
+      <c r="J20" s="13"/>
+      <c r="K20" s="13"/>
+      <c r="L20" s="13"/>
+      <c r="M20" s="14"/>
+      <c r="N20" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="O20" s="13"/>
+      <c r="P20" s="13"/>
+      <c r="Q20" s="13"/>
+      <c r="R20" s="14"/>
+      <c r="S20" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="T20" s="14"/>
+      <c r="U20" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="V20" s="14"/>
+    </row>
+    <row r="21" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B21" s="24"/>
+      <c r="C21" s="26"/>
+      <c r="D21" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="E21" s="25"/>
+      <c r="F21" s="25"/>
+      <c r="G21" s="26"/>
+      <c r="H21" s="24" t="s">
+        <v>10</v>
+      </c>
+      <c r="I21" s="25"/>
+      <c r="J21" s="25"/>
+      <c r="K21" s="25"/>
+      <c r="L21" s="25"/>
+      <c r="M21" s="26"/>
+      <c r="N21" s="24"/>
+      <c r="O21" s="25"/>
+      <c r="P21" s="25"/>
+      <c r="Q21" s="25"/>
+      <c r="R21" s="26"/>
+      <c r="S21" s="24"/>
+      <c r="T21" s="26"/>
+      <c r="U21" s="24"/>
+      <c r="V21" s="26"/>
+    </row>
+    <row r="22" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B22" s="42" t="s">
+        <v>3</v>
+      </c>
+      <c r="C22" s="43"/>
+      <c r="D22" s="44"/>
+      <c r="E22" s="45" t="s">
+        <v>22</v>
+      </c>
+      <c r="F22" s="46"/>
+      <c r="G22" s="46"/>
+      <c r="H22" s="46"/>
+      <c r="I22" s="46"/>
+      <c r="J22" s="46"/>
+      <c r="K22" s="46"/>
+      <c r="L22" s="46"/>
+      <c r="M22" s="47"/>
+      <c r="N22" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="O22" s="13"/>
+      <c r="P22" s="13"/>
+      <c r="Q22" s="13"/>
+      <c r="R22" s="13"/>
+      <c r="S22" s="13"/>
+      <c r="T22" s="13"/>
+      <c r="U22" s="13"/>
+      <c r="V22" s="14"/>
+    </row>
+    <row r="23" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B23" s="48" t="s">
+        <v>4</v>
+      </c>
+      <c r="C23" s="49"/>
+      <c r="D23" s="50"/>
+      <c r="E23" s="51" t="s">
+        <v>23</v>
+      </c>
+      <c r="F23" s="52"/>
+      <c r="G23" s="52"/>
+      <c r="H23" s="52"/>
+      <c r="I23" s="52"/>
+      <c r="J23" s="52"/>
+      <c r="K23" s="52"/>
+      <c r="L23" s="52"/>
+      <c r="M23" s="53"/>
+      <c r="N23" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="O23" s="16"/>
+      <c r="P23" s="16"/>
+      <c r="Q23" s="16"/>
+      <c r="R23" s="16"/>
+      <c r="S23" s="16"/>
+      <c r="T23" s="16"/>
+      <c r="U23" s="16"/>
+      <c r="V23" s="17"/>
+    </row>
+    <row r="24" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B24" s="48" t="s">
+        <v>5</v>
+      </c>
+      <c r="C24" s="49"/>
+      <c r="D24" s="50"/>
+      <c r="E24" s="51" t="s">
+        <v>13</v>
+      </c>
+      <c r="F24" s="52"/>
+      <c r="G24" s="52"/>
+      <c r="H24" s="52"/>
+      <c r="I24" s="52"/>
+      <c r="J24" s="52"/>
+      <c r="K24" s="52"/>
+      <c r="L24" s="52"/>
+      <c r="M24" s="53"/>
+      <c r="N24" s="18"/>
+      <c r="O24" s="19"/>
+      <c r="P24" s="19"/>
+      <c r="Q24" s="19"/>
+      <c r="R24" s="19"/>
+      <c r="S24" s="19"/>
+      <c r="T24" s="19"/>
+      <c r="U24" s="19"/>
+      <c r="V24" s="20"/>
+    </row>
+    <row r="25" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B25" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="C25" s="28"/>
+      <c r="D25" s="29"/>
+      <c r="E25" s="30"/>
+      <c r="F25" s="31"/>
+      <c r="G25" s="31"/>
+      <c r="H25" s="31"/>
+      <c r="I25" s="31"/>
+      <c r="J25" s="31"/>
+      <c r="K25" s="31"/>
+      <c r="L25" s="31"/>
+      <c r="M25" s="32"/>
+      <c r="N25" s="18"/>
+      <c r="O25" s="19"/>
+      <c r="P25" s="19"/>
+      <c r="Q25" s="19"/>
+      <c r="R25" s="19"/>
+      <c r="S25" s="19"/>
+      <c r="T25" s="19"/>
+      <c r="U25" s="19"/>
+      <c r="V25" s="20"/>
+    </row>
+    <row r="26" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B26" s="33" t="s">
+        <v>7</v>
+      </c>
+      <c r="C26" s="34"/>
+      <c r="D26" s="35"/>
+      <c r="E26" s="36"/>
+      <c r="F26" s="37"/>
+      <c r="G26" s="37"/>
+      <c r="H26" s="38"/>
+      <c r="I26" s="39" t="s">
+        <v>8</v>
+      </c>
+      <c r="J26" s="34"/>
+      <c r="K26" s="35"/>
+      <c r="L26" s="40"/>
+      <c r="M26" s="41"/>
+      <c r="N26" s="21"/>
+      <c r="O26" s="22"/>
+      <c r="P26" s="22"/>
+      <c r="Q26" s="22"/>
+      <c r="R26" s="22"/>
+      <c r="S26" s="22"/>
+      <c r="T26" s="22"/>
+      <c r="U26" s="22"/>
+      <c r="V26" s="23"/>
+    </row>
+    <row r="28" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B28" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
+      <c r="F28" s="1"/>
+      <c r="G28" s="1"/>
+      <c r="H28" s="1"/>
+      <c r="I28" s="1"/>
+      <c r="J28" s="1"/>
+      <c r="K28" s="1"/>
+      <c r="L28" s="1"/>
+      <c r="M28" s="1"/>
+      <c r="N28" s="1"/>
+      <c r="O28" s="1"/>
+      <c r="P28" s="1"/>
+      <c r="Q28" s="1"/>
+      <c r="R28" s="1"/>
+      <c r="S28" s="1"/>
+      <c r="T28" s="1"/>
+      <c r="U28" s="1"/>
+      <c r="V28" s="1"/>
+    </row>
+    <row r="29" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B29" s="2"/>
+      <c r="C29" s="3"/>
+      <c r="D29" s="3"/>
+      <c r="E29" s="3"/>
+      <c r="F29" s="3"/>
+      <c r="G29" s="3"/>
+      <c r="H29" s="3"/>
+      <c r="I29" s="3"/>
+      <c r="J29" s="3"/>
+      <c r="K29" s="3"/>
+      <c r="L29" s="3"/>
+      <c r="M29" s="3"/>
+      <c r="N29" s="3"/>
+      <c r="O29" s="3"/>
+      <c r="P29" s="3"/>
+      <c r="Q29" s="3"/>
+      <c r="R29" s="3"/>
+      <c r="S29" s="3"/>
+      <c r="T29" s="3"/>
+      <c r="U29" s="3"/>
+      <c r="V29" s="4"/>
+    </row>
+    <row r="30" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B30" s="5"/>
+      <c r="C30" s="6">
+        <v>1</v>
+      </c>
+      <c r="D30" t="s">
+        <v>24</v>
+      </c>
+      <c r="E30" s="7"/>
+      <c r="F30" s="7"/>
+      <c r="G30" s="7"/>
+      <c r="H30" s="7"/>
+      <c r="I30" s="7"/>
+      <c r="J30" s="7"/>
+      <c r="K30" s="7"/>
+      <c r="L30" s="7"/>
+      <c r="M30" s="7"/>
+      <c r="N30" s="7"/>
+      <c r="O30" s="7"/>
+      <c r="P30" s="7"/>
+      <c r="Q30" s="7"/>
+      <c r="R30" s="7"/>
+      <c r="S30" s="7"/>
+      <c r="T30" s="7"/>
+      <c r="U30" s="7"/>
+      <c r="V30" s="8"/>
+    </row>
+    <row r="31" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B31" s="5"/>
+      <c r="C31" s="6"/>
+      <c r="D31" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="E31" s="7"/>
+      <c r="F31" s="7"/>
+      <c r="G31" s="7"/>
+      <c r="H31" s="7"/>
+      <c r="I31" s="7"/>
+      <c r="J31" s="7"/>
+      <c r="K31" s="7"/>
+      <c r="L31" s="7"/>
+      <c r="M31" s="7"/>
+      <c r="N31" s="7"/>
+      <c r="O31" s="7"/>
+      <c r="P31" s="7"/>
+      <c r="Q31" s="7"/>
+      <c r="R31" s="7"/>
+      <c r="S31" s="7"/>
+      <c r="T31" s="7"/>
+      <c r="U31" s="7"/>
+      <c r="V31" s="8"/>
+    </row>
+    <row r="32" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B32" s="5"/>
+      <c r="C32" s="6"/>
+      <c r="D32" s="7"/>
+      <c r="E32" s="7"/>
+      <c r="F32" s="7"/>
+      <c r="G32" s="7"/>
+      <c r="H32" s="7"/>
+      <c r="I32" s="7"/>
+      <c r="J32" s="7"/>
+      <c r="K32" s="7"/>
+      <c r="L32" s="7"/>
+      <c r="M32" s="7"/>
+      <c r="N32" s="7"/>
+      <c r="O32" s="7"/>
+      <c r="P32" s="7"/>
+      <c r="Q32" s="7"/>
+      <c r="R32" s="7"/>
+      <c r="S32" s="7"/>
+      <c r="T32" s="7"/>
+      <c r="U32" s="7"/>
+      <c r="V32" s="8"/>
+    </row>
+    <row r="33" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B33" s="5"/>
+      <c r="C33" s="6"/>
+      <c r="D33" s="7"/>
+      <c r="E33" s="7"/>
+      <c r="F33" s="7"/>
+      <c r="G33" s="7"/>
+      <c r="H33" s="7"/>
+      <c r="I33" s="7"/>
+      <c r="J33" s="7"/>
+      <c r="K33" s="7"/>
+      <c r="L33" s="7"/>
+      <c r="M33" s="7"/>
+      <c r="N33" s="7"/>
+      <c r="O33" s="7"/>
+      <c r="P33" s="7"/>
+      <c r="Q33" s="7"/>
+      <c r="R33" s="7"/>
+      <c r="S33" s="7"/>
+      <c r="T33" s="7"/>
+      <c r="U33" s="7"/>
+      <c r="V33" s="8"/>
+    </row>
+    <row r="34" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B34" s="9"/>
+      <c r="C34" s="10"/>
+      <c r="D34" s="10"/>
+      <c r="E34" s="10"/>
+      <c r="F34" s="10"/>
+      <c r="G34" s="10"/>
+      <c r="H34" s="10"/>
+      <c r="I34" s="10"/>
+      <c r="J34" s="10"/>
+      <c r="K34" s="10"/>
+      <c r="L34" s="10"/>
+      <c r="M34" s="10"/>
+      <c r="N34" s="10"/>
+      <c r="O34" s="10"/>
+      <c r="P34" s="10"/>
+      <c r="Q34" s="10"/>
+      <c r="R34" s="10"/>
+      <c r="S34" s="10"/>
+      <c r="T34" s="10"/>
+      <c r="U34" s="10"/>
+      <c r="V34" s="11"/>
+    </row>
+  </sheetData>
+  <mergeCells count="26">
+    <mergeCell ref="U21:V21"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="D20:G20"/>
+    <mergeCell ref="H20:M20"/>
+    <mergeCell ref="N20:R20"/>
+    <mergeCell ref="S20:T20"/>
+    <mergeCell ref="U20:V20"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="D21:G21"/>
+    <mergeCell ref="H21:M21"/>
+    <mergeCell ref="N21:R21"/>
+    <mergeCell ref="S21:T21"/>
+    <mergeCell ref="N22:V22"/>
+    <mergeCell ref="B23:D23"/>
+    <mergeCell ref="E23:M23"/>
+    <mergeCell ref="N23:V26"/>
+    <mergeCell ref="B24:D24"/>
+    <mergeCell ref="E24:M24"/>
+    <mergeCell ref="B25:D25"/>
+    <mergeCell ref="E25:M25"/>
+    <mergeCell ref="B26:D26"/>
+    <mergeCell ref="E26:H26"/>
+    <mergeCell ref="I26:K26"/>
+    <mergeCell ref="L26:M26"/>
+    <mergeCell ref="B22:D22"/>
+    <mergeCell ref="E22:M22"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>